<commit_message>
add a new paper using graph attention network
</commit_message>
<xml_diff>
--- a/paperCounts.xlsx
+++ b/paperCounts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9420"/>
+    <workbookView windowWidth="19815" windowHeight="7860"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>论文题目</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t>实验结论</t>
+  </si>
+  <si>
+    <t>作用</t>
   </si>
   <si>
     <t>Training Language GANs from Scratch</t>
@@ -48,6 +51,9 @@
   <si>
     <t>如何在自然语言处理领域应用GAN,需要
 解决生成其不能生成离散数据的问题。论文主要提出三个解决办法，1.用于在每个时间步提供密集奖励的循环鉴别器 2.大批量的读取数据 3.鉴别器正规化</t>
+  </si>
+  <si>
+    <t>与研究领域关系不大，放弃</t>
   </si>
 </sst>
 </file>
@@ -55,9 +61,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
@@ -70,7 +76,60 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -83,68 +142,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -205,9 +205,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -222,19 +228,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -252,157 +408,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -413,6 +419,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -431,35 +452,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -505,11 +513,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -519,150 +525,153 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -991,21 +1000,22 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B1:G2"/>
+  <dimension ref="B1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelRow="1" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="7"/>
   <cols>
-    <col min="2" max="2" width="37.1111111111111" customWidth="1"/>
-    <col min="3" max="3" width="17.2222222222222" customWidth="1"/>
-    <col min="4" max="4" width="24.4444444444444" customWidth="1"/>
-    <col min="5" max="5" width="39.8888888888889" customWidth="1"/>
+    <col min="2" max="2" width="37.1083333333333" customWidth="1"/>
+    <col min="3" max="3" width="17.225" customWidth="1"/>
+    <col min="4" max="4" width="24.4416666666667" customWidth="1"/>
+    <col min="5" max="5" width="39.8916666666667" customWidth="1"/>
+    <col min="8" max="8" width="25.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7">
+    <row r="1" spans="2:8">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1024,19 +1034,25 @@
       <c r="G1" t="s">
         <v>5</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" ht="69" spans="2:5">
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
+    <row r="2" ht="71.25" spans="2:8">
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>9</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
complete the reading for this essay
</commit_message>
<xml_diff>
--- a/paperCounts.xlsx
+++ b/paperCounts.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>论文题目</t>
   </si>
@@ -54,6 +54,58 @@
   </si>
   <si>
     <t>与研究领域关系不大，放弃</t>
+  </si>
+  <si>
+    <t>Knowledge Graph Embedding via Graph
+Attenuated Attention Networks</t>
+  </si>
+  <si>
+    <t>IEEE Access 2019</t>
+  </si>
+  <si>
+    <t>图注意力衰减网络</t>
+  </si>
+  <si>
+    <t>讨论GATs的问题，论文提出了在GATs中加入
+注意力机制，同时引入了注意力衰减机制，以远近来对不同的邻居施以不同的权重</t>
+  </si>
+  <si>
+    <t>将测试方式分为两种：
+一种为原始(Raw),
+一种为过滤(Filter),
+原始的几位传统的测试方法，
+过滤的则是作者认为测试集中可能存在损坏的三元组，将其去掉之后在进行测试的方法</t>
+  </si>
+  <si>
+    <r>
+      <t>模型将减弱的注意力机制
+应用于关系和实体的表示，
+以获得实体和关系的新嵌入(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>虽然取得了较好的结果，但可信度不高</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>未来将图卷积神经网络与其它
+模型进行结合是可以作为参考</t>
   </si>
 </sst>
 </file>
@@ -61,12 +113,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,6 +127,49 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="等线"/>
@@ -82,27 +177,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -111,9 +185,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -124,29 +206,6 @@
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -182,6 +241,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="等线"/>
@@ -191,22 +258,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -216,6 +268,13 @@
       <color rgb="FF9C6500"/>
       <name val="等线"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -228,31 +287,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -264,67 +437,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -336,79 +455,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -419,6 +478,30 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -433,6 +516,30 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -471,203 +578,155 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -676,10 +735,22 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1000,59 +1071,84 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B1:H2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="2" outlineLevelCol="6"/>
   <cols>
-    <col min="2" max="2" width="37.1083333333333" customWidth="1"/>
-    <col min="3" max="3" width="17.225" customWidth="1"/>
-    <col min="4" max="4" width="24.4416666666667" customWidth="1"/>
-    <col min="5" max="5" width="39.8916666666667" customWidth="1"/>
-    <col min="8" max="8" width="25.375" customWidth="1"/>
+    <col min="1" max="1" width="37.1083333333333" customWidth="1"/>
+    <col min="2" max="2" width="17.225" customWidth="1"/>
+    <col min="3" max="3" width="24.4416666666667" customWidth="1"/>
+    <col min="4" max="4" width="39.8916666666667" customWidth="1"/>
+    <col min="5" max="5" width="25.375" customWidth="1"/>
+    <col min="6" max="6" width="24.5" customWidth="1"/>
+    <col min="7" max="7" width="25.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8">
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" ht="71.25" spans="2:8">
+    <row r="2" ht="71.25" spans="1:7">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="D2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="3" ht="104" customHeight="1" spans="1:7">
+      <c r="A3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>